<commit_message>
THANKS CHRIS - graphs and stats updated
</commit_message>
<xml_diff>
--- a/part2/all_stats/egress_analysis.xlsx
+++ b/part2/all_stats/egress_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\code\security_lab5\part2\all_stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C1B024-6AFB-4CAA-8A93-F1C0D11AF3E9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4F92B2-8E20-41BF-AA2A-A84C96965956}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10845" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -740,7 +740,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -756,17 +756,35 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99CCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99CCFF"/>
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF99FF66"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FF66"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -774,11 +792,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -790,10 +823,22 @@
     <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -867,6 +912,13 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FF99FF66"/>
+      <color rgb="FF99CCFF"/>
+      <color rgb="FFCC99FF"/>
+      <color rgb="FF33CCFF"/>
+      <color rgb="FF9933FF"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -913,7 +965,11 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
               <a:t>Packets Sent Count</a:t>
             </a:r>
           </a:p>
@@ -959,11 +1015,11 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>BRO</c:v>
+            <c:v>BRO Count</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="92D050"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1078,11 +1134,11 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>VPN</c:v>
+            <c:v>VPN Count</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:srgbClr val="FF0000"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1197,11 +1253,11 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>TOR</c:v>
+            <c:v>TOR Count</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3"/>
+              <a:srgbClr val="CC99FF"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1545,13 +1601,25 @@
       <c:spPr>
         <a:noFill/>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="2.8282439664232949E-2"/>
+          <c:y val="0.86631889763779524"/>
+          <c:w val="0.3666325431947699"/>
+          <c:h val="7.8125546806649168E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1598,10 +1666,7 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="tx1"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -1659,8 +1724,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Average Packet Length</a:t>
+              <a:rPr lang="en-US" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Average Packet Size</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1705,11 +1774,14 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>BRO</c:v>
+            <c:v>BRO Avg</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1718,7 +1790,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+            <c:numFmt formatCode="0" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1825,11 +1897,11 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>VPN</c:v>
+            <c:v>VPN Avg</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:srgbClr val="92D050"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1838,16 +1910,34 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:dLblPos val="inBase"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-CCF9-4DD9-ACF2-8514B51A095D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="0" sourceLinked="0"/>
             <c:spPr>
-              <a:noFill/>
-              <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
                 <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
@@ -1878,21 +1968,16 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+                <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
           </c:dLbls>
@@ -1945,11 +2030,11 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>TOR</c:v>
+            <c:v>TOR Avg</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3"/>
+              <a:srgbClr val="33CCFF"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1958,7 +2043,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+            <c:numFmt formatCode="0" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -2294,13 +2379,25 @@
       <c:spPr>
         <a:noFill/>
         <a:ln>
-          <a:noFill/>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="2.3173121785751913E-2"/>
+          <c:y val="0.87094852726742478"/>
+          <c:w val="0.30731536019443012"/>
+          <c:h val="6.0241360089656235E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2347,10 +2444,7 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="tx1"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -3468,16 +3562,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>23811</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3505,15 +3599,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>300037</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:colOff>595312</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>14286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>604837</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3840,16 +3934,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N331"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A307" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A321" sqref="A321:XFD321"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="6.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="6" customWidth="1"/>
-    <col min="4" max="1025" width="11.5703125"/>
+    <col min="4" max="4" width="11.5703125"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -8706,44 +8802,44 @@
         <v>2.11</v>
       </c>
     </row>
-    <row r="112" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="6" t="s">
+    <row r="112" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="B112" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C112" s="6">
-        <v>0</v>
-      </c>
-      <c r="D112" s="7">
-        <v>0</v>
-      </c>
-      <c r="F112" s="7" t="s">
+      <c r="B112" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C112" s="12">
+        <v>0</v>
+      </c>
+      <c r="D112" s="13">
+        <v>0</v>
+      </c>
+      <c r="F112" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G112" s="7">
+      <c r="G112" s="13">
         <v>22</v>
       </c>
-      <c r="H112" s="7">
+      <c r="H112" s="13">
         <v>831.14</v>
       </c>
-      <c r="I112" s="7">
+      <c r="I112" s="13">
         <v>54</v>
       </c>
-      <c r="J112" s="7">
+      <c r="J112" s="13">
         <v>1375</v>
       </c>
-      <c r="K112" s="7">
+      <c r="K112" s="13">
         <v>0.19389999999999999</v>
       </c>
-      <c r="L112" s="8" t="s">
+      <c r="L112" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="M112" s="7">
+      <c r="M112" s="13">
         <v>0.21</v>
       </c>
-      <c r="N112" s="7">
+      <c r="N112" s="13">
         <v>0</v>
       </c>
     </row>
@@ -9187,44 +9283,44 @@
         <v>20</v>
       </c>
     </row>
-    <row r="123" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="6" t="s">
+    <row r="123" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B123" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C123" s="6">
-        <v>1</v>
-      </c>
-      <c r="D123" s="7">
-        <v>0</v>
-      </c>
-      <c r="F123" s="7" t="s">
+      <c r="B123" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C123" s="15">
+        <v>1</v>
+      </c>
+      <c r="D123" s="16">
+        <v>0</v>
+      </c>
+      <c r="F123" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G123" s="7">
+      <c r="G123" s="16">
         <v>378</v>
       </c>
-      <c r="H123" s="7">
+      <c r="H123" s="16">
         <v>786.88</v>
       </c>
-      <c r="I123" s="7">
+      <c r="I123" s="16">
         <v>54</v>
       </c>
-      <c r="J123" s="7">
+      <c r="J123" s="16">
         <v>1514</v>
       </c>
-      <c r="K123" s="7">
+      <c r="K123" s="16">
         <v>0.33779999999999999</v>
       </c>
-      <c r="L123" s="8" t="s">
+      <c r="L123" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="M123" s="7">
+      <c r="M123" s="16">
         <v>1.8</v>
       </c>
-      <c r="N123" s="7">
+      <c r="N123" s="16">
         <v>1.1160000000000001</v>
       </c>
     </row>
@@ -9668,44 +9764,44 @@
         <v>20</v>
       </c>
     </row>
-    <row r="134" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="6" t="s">
+    <row r="134" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B134" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C134" s="6">
+      <c r="B134" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C134" s="15">
         <v>2</v>
       </c>
-      <c r="D134" s="7">
-        <v>0</v>
-      </c>
-      <c r="F134" s="7" t="s">
+      <c r="D134" s="16">
+        <v>0</v>
+      </c>
+      <c r="F134" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G134" s="7">
+      <c r="G134" s="16">
         <v>357</v>
       </c>
-      <c r="H134" s="7">
+      <c r="H134" s="16">
         <v>865</v>
       </c>
-      <c r="I134" s="7">
+      <c r="I134" s="16">
         <v>54</v>
       </c>
-      <c r="J134" s="7">
+      <c r="J134" s="16">
         <v>1514</v>
       </c>
-      <c r="K134" s="7">
+      <c r="K134" s="16">
         <v>0.69199999999999995</v>
       </c>
-      <c r="L134" s="8" t="s">
+      <c r="L134" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="M134" s="7">
+      <c r="M134" s="16">
         <v>1.92</v>
       </c>
-      <c r="N134" s="7">
+      <c r="N134" s="16">
         <v>1.375</v>
       </c>
     </row>
@@ -10149,44 +10245,44 @@
         <v>20</v>
       </c>
     </row>
-    <row r="145" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="6" t="s">
+    <row r="145" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B145" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C145" s="6">
+      <c r="B145" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C145" s="15">
         <v>3</v>
       </c>
-      <c r="D145" s="7">
-        <v>0</v>
-      </c>
-      <c r="F145" s="7" t="s">
+      <c r="D145" s="16">
+        <v>0</v>
+      </c>
+      <c r="F145" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G145" s="7">
+      <c r="G145" s="16">
         <v>310</v>
       </c>
-      <c r="H145" s="7">
+      <c r="H145" s="16">
         <v>923.58</v>
       </c>
-      <c r="I145" s="7">
+      <c r="I145" s="16">
         <v>54</v>
       </c>
-      <c r="J145" s="7">
+      <c r="J145" s="16">
         <v>1514</v>
       </c>
-      <c r="K145" s="7">
+      <c r="K145" s="16">
         <v>1.0375000000000001</v>
       </c>
-      <c r="L145" s="8" t="s">
+      <c r="L145" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="M145" s="7">
+      <c r="M145" s="16">
         <v>1.83</v>
       </c>
-      <c r="N145" s="7">
+      <c r="N145" s="16">
         <v>0.18</v>
       </c>
     </row>
@@ -10630,44 +10726,44 @@
         <v>20</v>
       </c>
     </row>
-    <row r="156" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A156" s="6" t="s">
+    <row r="156" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B156" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C156" s="6">
+      <c r="B156" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C156" s="15">
         <v>4</v>
       </c>
-      <c r="D156" s="7">
-        <v>0</v>
-      </c>
-      <c r="F156" s="7" t="s">
+      <c r="D156" s="16">
+        <v>0</v>
+      </c>
+      <c r="F156" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G156" s="7">
+      <c r="G156" s="16">
         <v>308</v>
       </c>
-      <c r="H156" s="7">
+      <c r="H156" s="16">
         <v>929.06</v>
       </c>
-      <c r="I156" s="7">
+      <c r="I156" s="16">
         <v>54</v>
       </c>
-      <c r="J156" s="7">
+      <c r="J156" s="16">
         <v>1514</v>
       </c>
-      <c r="K156" s="7">
+      <c r="K156" s="16">
         <v>1.0387999999999999</v>
       </c>
-      <c r="L156" s="8" t="s">
+      <c r="L156" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="M156" s="7">
+      <c r="M156" s="16">
         <v>1.86</v>
       </c>
-      <c r="N156" s="7">
+      <c r="N156" s="16">
         <v>1.0149999999999999</v>
       </c>
     </row>
@@ -11111,44 +11207,44 @@
         <v>20</v>
       </c>
     </row>
-    <row r="167" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A167" s="6" t="s">
+    <row r="167" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A167" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B167" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C167" s="6">
+      <c r="B167" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C167" s="15">
         <v>5</v>
       </c>
-      <c r="D167" s="7">
-        <v>0</v>
-      </c>
-      <c r="F167" s="7" t="s">
+      <c r="D167" s="16">
+        <v>0</v>
+      </c>
+      <c r="F167" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G167" s="7">
+      <c r="G167" s="16">
         <v>355</v>
       </c>
-      <c r="H167" s="7">
+      <c r="H167" s="16">
         <v>822.34</v>
       </c>
-      <c r="I167" s="7">
+      <c r="I167" s="16">
         <v>54</v>
       </c>
-      <c r="J167" s="7">
+      <c r="J167" s="16">
         <v>1514</v>
       </c>
-      <c r="K167" s="7">
+      <c r="K167" s="16">
         <v>0.86519999999999997</v>
       </c>
-      <c r="L167" s="8" t="s">
+      <c r="L167" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="M167" s="7">
+      <c r="M167" s="16">
         <v>1.84</v>
       </c>
-      <c r="N167" s="7">
+      <c r="N167" s="16">
         <v>0.30199999999999999</v>
       </c>
     </row>
@@ -11592,44 +11688,44 @@
         <v>20</v>
       </c>
     </row>
-    <row r="178" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A178" s="6" t="s">
+    <row r="178" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A178" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B178" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C178" s="6">
+      <c r="B178" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C178" s="15">
         <v>6</v>
       </c>
-      <c r="D178" s="7">
-        <v>0</v>
-      </c>
-      <c r="F178" s="7" t="s">
+      <c r="D178" s="16">
+        <v>0</v>
+      </c>
+      <c r="F178" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G178" s="7">
+      <c r="G178" s="16">
         <v>314</v>
       </c>
-      <c r="H178" s="7">
+      <c r="H178" s="16">
         <v>913.37</v>
       </c>
-      <c r="I178" s="7">
+      <c r="I178" s="16">
         <v>54</v>
       </c>
-      <c r="J178" s="7">
+      <c r="J178" s="16">
         <v>1514</v>
       </c>
-      <c r="K178" s="7">
+      <c r="K178" s="16">
         <v>0.33600000000000002</v>
       </c>
-      <c r="L178" s="8" t="s">
+      <c r="L178" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="M178" s="7">
+      <c r="M178" s="16">
         <v>1.83</v>
       </c>
-      <c r="N178" s="7">
+      <c r="N178" s="16">
         <v>0.153</v>
       </c>
     </row>
@@ -12073,44 +12169,44 @@
         <v>20</v>
       </c>
     </row>
-    <row r="189" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A189" s="6" t="s">
+    <row r="189" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A189" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B189" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C189" s="6">
+      <c r="B189" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C189" s="15">
         <v>7</v>
       </c>
-      <c r="D189" s="7">
-        <v>0</v>
-      </c>
-      <c r="F189" s="7" t="s">
+      <c r="D189" s="16">
+        <v>0</v>
+      </c>
+      <c r="F189" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G189" s="7">
+      <c r="G189" s="16">
         <v>376</v>
       </c>
-      <c r="H189" s="7">
+      <c r="H189" s="16">
         <v>792.36</v>
       </c>
-      <c r="I189" s="7">
+      <c r="I189" s="16">
         <v>54</v>
       </c>
-      <c r="J189" s="7">
+      <c r="J189" s="16">
         <v>1514</v>
       </c>
-      <c r="K189" s="7">
+      <c r="K189" s="16">
         <v>0.19769999999999999</v>
       </c>
-      <c r="L189" s="8" t="s">
+      <c r="L189" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="M189" s="7">
+      <c r="M189" s="16">
         <v>1.71</v>
       </c>
-      <c r="N189" s="7">
+      <c r="N189" s="16">
         <v>1.774</v>
       </c>
     </row>
@@ -12554,44 +12650,44 @@
         <v>20</v>
       </c>
     </row>
-    <row r="200" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A200" s="6" t="s">
+    <row r="200" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A200" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B200" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C200" s="6">
+      <c r="B200" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C200" s="15">
         <v>8</v>
       </c>
-      <c r="D200" s="7">
-        <v>0</v>
-      </c>
-      <c r="F200" s="7" t="s">
+      <c r="D200" s="16">
+        <v>0</v>
+      </c>
+      <c r="F200" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G200" s="7">
+      <c r="G200" s="16">
         <v>323</v>
       </c>
-      <c r="H200" s="7">
+      <c r="H200" s="16">
         <v>889.21</v>
       </c>
-      <c r="I200" s="7">
+      <c r="I200" s="16">
         <v>54</v>
       </c>
-      <c r="J200" s="7">
+      <c r="J200" s="16">
         <v>1514</v>
       </c>
-      <c r="K200" s="7">
+      <c r="K200" s="16">
         <v>0.1163</v>
       </c>
-      <c r="L200" s="8" t="s">
+      <c r="L200" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="M200" s="7">
+      <c r="M200" s="16">
         <v>2.14</v>
       </c>
-      <c r="N200" s="7">
+      <c r="N200" s="16">
         <v>0.13600000000000001</v>
       </c>
     </row>
@@ -13035,44 +13131,44 @@
         <v>20</v>
       </c>
     </row>
-    <row r="211" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A211" s="6" t="s">
+    <row r="211" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A211" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B211" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C211" s="6">
+      <c r="B211" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C211" s="15">
         <v>9</v>
       </c>
-      <c r="D211" s="7">
-        <v>0</v>
-      </c>
-      <c r="F211" s="7" t="s">
+      <c r="D211" s="16">
+        <v>0</v>
+      </c>
+      <c r="F211" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G211" s="7">
+      <c r="G211" s="16">
         <v>309</v>
       </c>
-      <c r="H211" s="7">
+      <c r="H211" s="16">
         <v>927.01</v>
       </c>
-      <c r="I211" s="7">
+      <c r="I211" s="16">
         <v>46</v>
       </c>
-      <c r="J211" s="7">
+      <c r="J211" s="16">
         <v>1514</v>
       </c>
-      <c r="K211" s="7">
+      <c r="K211" s="16">
         <v>0.61729999999999996</v>
       </c>
-      <c r="L211" s="8" t="s">
+      <c r="L211" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="M211" s="7">
+      <c r="M211" s="16">
         <v>1.86</v>
       </c>
-      <c r="N211" s="7">
+      <c r="N211" s="16">
         <v>1.05</v>
       </c>
     </row>
@@ -13516,44 +13612,44 @@
         <v>20</v>
       </c>
     </row>
-    <row r="222" spans="1:14" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A222" s="11" t="s">
+    <row r="222" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A222" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="B222" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C222" s="11">
-        <v>0</v>
-      </c>
-      <c r="D222" s="12">
-        <v>0</v>
-      </c>
-      <c r="F222" s="12" t="s">
+      <c r="B222" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C222" s="18">
+        <v>0</v>
+      </c>
+      <c r="D222" s="19">
+        <v>0</v>
+      </c>
+      <c r="F222" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="G222" s="12">
+      <c r="G222" s="19">
         <v>145</v>
       </c>
-      <c r="H222" s="12">
+      <c r="H222" s="19">
         <v>1482.42</v>
       </c>
-      <c r="I222" s="12">
+      <c r="I222" s="19">
         <v>56</v>
       </c>
-      <c r="J222" s="12">
+      <c r="J222" s="19">
         <v>13196</v>
       </c>
-      <c r="K222" s="12">
+      <c r="K222" s="19">
         <v>8.5699999999999998E-2</v>
       </c>
-      <c r="L222" s="13" t="s">
+      <c r="L222" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="M222" s="12">
+      <c r="M222" s="19">
         <v>0.59</v>
       </c>
-      <c r="N222" s="12">
+      <c r="N222" s="19">
         <v>1.5049999999999999</v>
       </c>
     </row>
@@ -13997,44 +14093,44 @@
         <v>1.399</v>
       </c>
     </row>
-    <row r="233" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A233" s="6" t="s">
+    <row r="233" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A233" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="B233" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C233" s="6">
-        <v>1</v>
-      </c>
-      <c r="D233" s="7">
-        <v>0</v>
-      </c>
-      <c r="F233" s="7" t="s">
+      <c r="B233" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C233" s="18">
+        <v>1</v>
+      </c>
+      <c r="D233" s="21">
+        <v>0</v>
+      </c>
+      <c r="F233" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G233" s="7">
+      <c r="G233" s="21">
         <v>231</v>
       </c>
-      <c r="H233" s="7">
+      <c r="H233" s="21">
         <v>1387.03</v>
       </c>
-      <c r="I233" s="7">
+      <c r="I233" s="21">
         <v>56</v>
       </c>
-      <c r="J233" s="7">
+      <c r="J233" s="21">
         <v>21956</v>
       </c>
-      <c r="K233" s="7">
+      <c r="K233" s="21">
         <v>8.2699999999999996E-2</v>
       </c>
-      <c r="L233" s="8" t="s">
+      <c r="L233" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="M233" s="7">
+      <c r="M233" s="21">
         <v>0.75</v>
       </c>
-      <c r="N233" s="7">
+      <c r="N233" s="21">
         <v>2.6360000000000001</v>
       </c>
     </row>
@@ -14478,44 +14574,44 @@
         <v>2.58</v>
       </c>
     </row>
-    <row r="244" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A244" s="6" t="s">
+    <row r="244" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A244" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="B244" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C244" s="6">
+      <c r="B244" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C244" s="18">
         <v>2</v>
       </c>
-      <c r="D244" s="7">
-        <v>0</v>
-      </c>
-      <c r="F244" s="7" t="s">
+      <c r="D244" s="21">
+        <v>0</v>
+      </c>
+      <c r="F244" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G244" s="7">
+      <c r="G244" s="21">
         <v>243</v>
       </c>
-      <c r="H244" s="7">
+      <c r="H244" s="21">
         <v>1308.4000000000001</v>
       </c>
-      <c r="I244" s="7">
+      <c r="I244" s="21">
         <v>56</v>
       </c>
-      <c r="J244" s="7">
+      <c r="J244" s="21">
         <v>23416</v>
       </c>
-      <c r="K244" s="7">
+      <c r="K244" s="21">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="L244" s="8" t="s">
+      <c r="L244" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="M244" s="7">
+      <c r="M244" s="21">
         <v>0.72</v>
       </c>
-      <c r="N244" s="7">
+      <c r="N244" s="21">
         <v>2.976</v>
       </c>
     </row>
@@ -14959,44 +15055,44 @@
         <v>2.976</v>
       </c>
     </row>
-    <row r="255" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A255" s="6" t="s">
+    <row r="255" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A255" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="B255" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C255" s="6">
+      <c r="B255" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C255" s="18">
         <v>3</v>
       </c>
-      <c r="D255" s="7">
-        <v>0</v>
-      </c>
-      <c r="F255" s="7" t="s">
+      <c r="D255" s="21">
+        <v>0</v>
+      </c>
+      <c r="F255" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G255" s="7">
+      <c r="G255" s="21">
         <v>197</v>
       </c>
-      <c r="H255" s="7">
+      <c r="H255" s="21">
         <v>1619.34</v>
       </c>
-      <c r="I255" s="7">
+      <c r="I255" s="21">
         <v>56</v>
       </c>
-      <c r="J255" s="7">
+      <c r="J255" s="21">
         <v>17576</v>
       </c>
-      <c r="K255" s="7">
+      <c r="K255" s="21">
         <v>6.4699999999999994E-2</v>
       </c>
-      <c r="L255" s="8" t="s">
+      <c r="L255" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="M255" s="7">
+      <c r="M255" s="21">
         <v>0.46</v>
       </c>
-      <c r="N255" s="7">
+      <c r="N255" s="21">
         <v>2.8119999999999998</v>
       </c>
     </row>
@@ -15440,44 +15536,44 @@
         <v>2.6779999999999999</v>
       </c>
     </row>
-    <row r="266" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A266" s="6" t="s">
+    <row r="266" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A266" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="B266" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C266" s="6">
+      <c r="B266" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C266" s="18">
         <v>4</v>
       </c>
-      <c r="D266" s="7">
-        <v>0</v>
-      </c>
-      <c r="F266" s="7" t="s">
+      <c r="D266" s="21">
+        <v>0</v>
+      </c>
+      <c r="F266" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G266" s="7">
+      <c r="G266" s="21">
         <v>237</v>
       </c>
-      <c r="H266" s="7">
+      <c r="H266" s="21">
         <v>1350.95</v>
       </c>
-      <c r="I266" s="7">
+      <c r="I266" s="21">
         <v>56</v>
       </c>
-      <c r="J266" s="7">
+      <c r="J266" s="21">
         <v>8816</v>
       </c>
-      <c r="K266" s="7">
+      <c r="K266" s="21">
         <v>6.4100000000000004E-2</v>
       </c>
-      <c r="L266" s="8" t="s">
+      <c r="L266" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="M266" s="7">
+      <c r="M266" s="21">
         <v>0.61</v>
       </c>
-      <c r="N266" s="7">
+      <c r="N266" s="21">
         <v>3.36</v>
       </c>
     </row>
@@ -15921,44 +16017,44 @@
         <v>3.387</v>
       </c>
     </row>
-    <row r="277" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A277" s="6" t="s">
+    <row r="277" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A277" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="B277" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C277" s="6">
+      <c r="B277" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C277" s="18">
         <v>5</v>
       </c>
-      <c r="D277" s="7">
-        <v>0</v>
-      </c>
-      <c r="F277" s="7" t="s">
+      <c r="D277" s="21">
+        <v>0</v>
+      </c>
+      <c r="F277" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G277" s="7">
+      <c r="G277" s="21">
         <v>238</v>
       </c>
-      <c r="H277" s="7">
+      <c r="H277" s="21">
         <v>1332.38</v>
       </c>
-      <c r="I277" s="7">
+      <c r="I277" s="21">
         <v>56</v>
       </c>
-      <c r="J277" s="7">
+      <c r="J277" s="21">
         <v>11736</v>
       </c>
-      <c r="K277" s="7">
+      <c r="K277" s="21">
         <v>7.22E-2</v>
       </c>
-      <c r="L277" s="8" t="s">
+      <c r="L277" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="M277" s="7">
+      <c r="M277" s="21">
         <v>0.84</v>
       </c>
-      <c r="N277" s="7">
+      <c r="N277" s="21">
         <v>3.0830000000000002</v>
       </c>
     </row>
@@ -16402,44 +16498,44 @@
         <v>2.9489999999999998</v>
       </c>
     </row>
-    <row r="288" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A288" s="6" t="s">
+    <row r="288" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A288" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="B288" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C288" s="6">
+      <c r="B288" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C288" s="18">
         <v>6</v>
       </c>
-      <c r="D288" s="7">
-        <v>0</v>
-      </c>
-      <c r="F288" s="7" t="s">
+      <c r="D288" s="21">
+        <v>0</v>
+      </c>
+      <c r="F288" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G288" s="7">
+      <c r="G288" s="21">
         <v>246</v>
       </c>
-      <c r="H288" s="7">
+      <c r="H288" s="21">
         <v>1306.56</v>
       </c>
-      <c r="I288" s="7">
+      <c r="I288" s="21">
         <v>56</v>
       </c>
-      <c r="J288" s="7">
+      <c r="J288" s="21">
         <v>8816</v>
       </c>
-      <c r="K288" s="7">
+      <c r="K288" s="21">
         <v>8.0199999999999994E-2</v>
       </c>
-      <c r="L288" s="8" t="s">
+      <c r="L288" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="M288" s="7">
+      <c r="M288" s="21">
         <v>0.69</v>
       </c>
-      <c r="N288" s="7">
+      <c r="N288" s="21">
         <v>2.86</v>
       </c>
     </row>
@@ -16883,44 +16979,44 @@
         <v>2.8610000000000002</v>
       </c>
     </row>
-    <row r="299" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A299" s="6" t="s">
+    <row r="299" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A299" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="B299" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C299" s="6">
+      <c r="B299" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C299" s="18">
         <v>7</v>
       </c>
-      <c r="D299" s="7">
-        <v>0</v>
-      </c>
-      <c r="F299" s="7" t="s">
+      <c r="D299" s="21">
+        <v>0</v>
+      </c>
+      <c r="F299" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G299" s="7">
+      <c r="G299" s="21">
         <v>242</v>
       </c>
-      <c r="H299" s="7">
+      <c r="H299" s="21">
         <v>1316.47</v>
       </c>
-      <c r="I299" s="7">
+      <c r="I299" s="21">
         <v>56</v>
       </c>
-      <c r="J299" s="7">
+      <c r="J299" s="21">
         <v>8816</v>
       </c>
-      <c r="K299" s="7">
+      <c r="K299" s="21">
         <v>7.0400000000000004E-2</v>
       </c>
-      <c r="L299" s="8" t="s">
+      <c r="L299" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="M299" s="7">
+      <c r="M299" s="21">
         <v>0.48</v>
       </c>
-      <c r="N299" s="7">
+      <c r="N299" s="21">
         <v>3.1059999999999999</v>
       </c>
     </row>
@@ -17364,44 +17460,44 @@
         <v>3.21</v>
       </c>
     </row>
-    <row r="310" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A310" s="6" t="s">
+    <row r="310" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A310" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="B310" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C310" s="6">
+      <c r="B310" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C310" s="18">
         <v>8</v>
       </c>
-      <c r="D310" s="7">
-        <v>0</v>
-      </c>
-      <c r="F310" s="7" t="s">
+      <c r="D310" s="21">
+        <v>0</v>
+      </c>
+      <c r="F310" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G310" s="7">
+      <c r="G310" s="21">
         <v>263</v>
       </c>
-      <c r="H310" s="7">
+      <c r="H310" s="21">
         <v>1229.48</v>
       </c>
-      <c r="I310" s="7">
+      <c r="I310" s="21">
         <v>56</v>
       </c>
-      <c r="J310" s="7">
+      <c r="J310" s="21">
         <v>8816</v>
       </c>
-      <c r="K310" s="7">
+      <c r="K310" s="21">
         <v>7.7299999999999994E-2</v>
       </c>
-      <c r="L310" s="8" t="s">
+      <c r="L310" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="M310" s="7">
+      <c r="M310" s="21">
         <v>0.72</v>
       </c>
-      <c r="N310" s="7">
+      <c r="N310" s="21">
         <v>2.92</v>
       </c>
     </row>
@@ -17845,44 +17941,44 @@
         <v>3.0550000000000002</v>
       </c>
     </row>
-    <row r="321" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A321" s="6" t="s">
+    <row r="321" spans="1:14" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A321" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="B321" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C321" s="6">
+      <c r="B321" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C321" s="18">
         <v>9</v>
       </c>
-      <c r="D321" s="7">
-        <v>0</v>
-      </c>
-      <c r="F321" s="7" t="s">
+      <c r="D321" s="21">
+        <v>0</v>
+      </c>
+      <c r="F321" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G321" s="7">
+      <c r="G321" s="21">
         <v>252</v>
       </c>
-      <c r="H321" s="7">
+      <c r="H321" s="21">
         <v>1276.3900000000001</v>
       </c>
-      <c r="I321" s="7">
+      <c r="I321" s="21">
         <v>56</v>
       </c>
-      <c r="J321" s="7">
+      <c r="J321" s="21">
         <v>7356</v>
       </c>
-      <c r="K321" s="7">
+      <c r="K321" s="21">
         <v>5.67E-2</v>
       </c>
-      <c r="L321" s="8" t="s">
+      <c r="L321" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="M321" s="7">
+      <c r="M321" s="21">
         <v>0.79</v>
       </c>
-      <c r="N321" s="7">
+      <c r="N321" s="21">
         <v>4.1980000000000004</v>
       </c>
     </row>
@@ -18341,1286 +18437,1317 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{844ACC77-EE99-4738-A404-ECA8DAD0342C}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H12" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+    <sheetView tabSelected="1" topLeftCell="H25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA19" sqref="AA19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="14" t="s">
+    <row r="1" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="23" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="B2" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="24">
+        <v>0</v>
+      </c>
+      <c r="D2" s="24">
+        <v>0</v>
+      </c>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="24">
         <v>65</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="24">
         <v>3403.65</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="24">
         <v>56</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="24">
         <v>24876</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="24">
         <v>1.72E-2</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="24">
         <v>0.42</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="24">
         <v>3.746</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="B3" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="24">
+        <v>1</v>
+      </c>
+      <c r="D3" s="24">
+        <v>0</v>
+      </c>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="24">
         <v>88</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="24">
         <v>2607.3200000000002</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="24">
         <v>56</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="24">
         <v>41236</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="24">
         <v>0.1023</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="24">
         <v>0.26</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="24">
         <v>1.7330000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="24">
         <v>2</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="D4" s="24">
+        <v>0</v>
+      </c>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="24">
         <v>202</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="24">
         <v>1376.57</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="24">
         <v>56</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="24">
         <v>14656</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="24">
         <v>0.35210000000000002</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="24">
         <v>0.77</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="24">
         <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="24">
         <v>3</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="D5" s="24">
+        <v>0</v>
+      </c>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="24">
         <v>214</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="24">
         <v>1306.8900000000001</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="24">
         <v>56</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="24">
         <v>19036</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="24">
         <v>0.39119999999999999</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="24">
         <v>0.78</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="24">
         <v>0.20200000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="24">
         <v>4</v>
       </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="D6" s="24">
+        <v>0</v>
+      </c>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="24">
         <v>233</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="24">
         <v>1231.55</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="24">
         <v>56</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="24">
         <v>11736</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="24">
         <v>0.3196</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="24">
         <v>0.99</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="24">
         <v>0.61699999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7">
+      <c r="B7" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="24">
         <v>5</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="D7" s="24">
+        <v>0</v>
+      </c>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="24">
         <v>226</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="24">
         <v>1239.2</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="24">
         <v>56</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="24">
         <v>16116</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="24">
         <v>0.50629999999999997</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="24">
         <v>0.95</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="24">
         <v>1.7250000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8">
+      <c r="B8" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="24">
         <v>6</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="D8" s="24">
+        <v>0</v>
+      </c>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="24">
         <v>212</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="24">
         <v>1317.99</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="24">
         <v>56</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="24">
         <v>13196</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="24">
         <v>0.32950000000000002</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="24">
         <v>0.89</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="24">
         <v>0.51300000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9">
+      <c r="B9" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="24">
         <v>7</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="D9" s="24">
+        <v>0</v>
+      </c>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="24">
         <v>84</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="24">
         <v>534.35</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="24">
         <v>56</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="24">
         <v>11736</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="24">
         <v>0.1216</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="24">
         <v>0.37</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="24">
         <v>0.02</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10">
+      <c r="B10" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="24">
         <v>8</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="D10" s="24">
+        <v>0</v>
+      </c>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="24">
         <v>225</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="24">
         <v>1244.95</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="24">
         <v>56</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="24">
         <v>13196</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="24">
         <v>0.46179999999999999</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="24">
         <v>0.8</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="24">
         <v>0.36499999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11">
+      <c r="B11" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="24">
         <v>9</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="F11" t="s">
+      <c r="D11" s="24">
+        <v>0</v>
+      </c>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="24">
         <v>211</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="24">
         <v>1324.59</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="24">
         <v>56</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="24">
         <v>11736</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="24">
         <v>0.40579999999999999</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="24">
         <v>0.73</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="24">
         <v>2.0569999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="B12" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="25">
+        <v>0</v>
+      </c>
+      <c r="D12" s="25">
+        <v>0</v>
+      </c>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="25">
         <v>22</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="25">
         <v>831.14</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="25">
         <v>54</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="25">
         <v>1375</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="25">
         <v>0.19389999999999999</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="25">
         <v>0.21</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="25">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="B13" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="25">
+        <v>1</v>
+      </c>
+      <c r="D13" s="25">
+        <v>0</v>
+      </c>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="25">
         <v>378</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="25">
         <v>786.88</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="25">
         <v>54</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="25">
         <v>1514</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="25">
         <v>0.33779999999999999</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="25">
         <v>1.8</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="25">
         <v>1.1160000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14">
+      <c r="B14" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="25">
         <v>2</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="D14" s="25">
+        <v>0</v>
+      </c>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="25">
         <v>357</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="25">
         <v>865</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="25">
         <v>54</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="25">
         <v>1514</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="25">
         <v>0.69199999999999995</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="25">
         <v>1.92</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="25">
         <v>1.375</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15">
+      <c r="B15" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="25">
         <v>3</v>
       </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="D15" s="25">
+        <v>0</v>
+      </c>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="25">
         <v>310</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="25">
         <v>923.58</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="25">
         <v>54</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="25">
         <v>1514</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="25">
         <v>1.0375000000000001</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L15" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="25">
         <v>1.83</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="25">
         <v>0.18</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="B16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16">
+      <c r="B16" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="25">
         <v>4</v>
       </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="D16" s="25">
+        <v>0</v>
+      </c>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="25">
         <v>308</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="25">
         <v>929.06</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="25">
         <v>54</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="25">
         <v>1514</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="25">
         <v>1.0387999999999999</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L16" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="25">
         <v>1.86</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="25">
         <v>1.0149999999999999</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="B17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17">
+      <c r="B17" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="25">
         <v>5</v>
       </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="D17" s="25">
+        <v>0</v>
+      </c>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="25">
         <v>355</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="25">
         <v>822.34</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="25">
         <v>54</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="25">
         <v>1514</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="25">
         <v>0.86519999999999997</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L17" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="25">
         <v>1.84</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="25">
         <v>0.30199999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="B18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18">
+      <c r="B18" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="25">
         <v>6</v>
       </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="D18" s="25">
+        <v>0</v>
+      </c>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="25">
         <v>314</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="25">
         <v>913.37</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="25">
         <v>54</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="25">
         <v>1514</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="25">
         <v>0.33600000000000002</v>
       </c>
-      <c r="L18" t="s">
+      <c r="L18" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="25">
         <v>1.83</v>
       </c>
-      <c r="N18">
+      <c r="N18" s="25">
         <v>0.153</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19">
+      <c r="B19" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="25">
         <v>7</v>
       </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="D19" s="25">
+        <v>0</v>
+      </c>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="25">
         <v>376</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="25">
         <v>792.36</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="25">
         <v>54</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="25">
         <v>1514</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="25">
         <v>0.19769999999999999</v>
       </c>
-      <c r="L19" t="s">
+      <c r="L19" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="25">
         <v>1.71</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="25">
         <v>1.774</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="B20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20">
+      <c r="B20" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="25">
         <v>8</v>
       </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="D20" s="25">
+        <v>0</v>
+      </c>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="25">
         <v>323</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="25">
         <v>889.21</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="25">
         <v>54</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="25">
         <v>1514</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="25">
         <v>0.1163</v>
       </c>
-      <c r="L20" t="s">
+      <c r="L20" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="25">
         <v>2.14</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="25">
         <v>0.13600000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="B21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21">
+      <c r="B21" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="25">
         <v>9</v>
       </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="F21" t="s">
+      <c r="D21" s="25">
+        <v>0</v>
+      </c>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="25">
         <v>309</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="25">
         <v>927.01</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="25">
         <v>46</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="25">
         <v>1514</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="25">
         <v>0.61729999999999996</v>
       </c>
-      <c r="L21" t="s">
+      <c r="L21" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="25">
         <v>1.86</v>
       </c>
-      <c r="N21">
+      <c r="N21" s="25">
         <v>1.05</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A22" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="B22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="B22" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="26">
+        <v>0</v>
+      </c>
+      <c r="D22" s="26">
+        <v>0</v>
+      </c>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="26">
         <v>145</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="26">
         <v>1482.42</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="26">
         <v>56</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="26">
         <v>13196</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="26">
         <v>8.5699999999999998E-2</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L22" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="26">
         <v>0.59</v>
       </c>
-      <c r="N22">
+      <c r="N22" s="26">
         <v>1.5049999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="A23" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="B23" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="F23" t="s">
+      <c r="B23" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="26">
+        <v>1</v>
+      </c>
+      <c r="D23" s="26">
+        <v>0</v>
+      </c>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="26">
         <v>231</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="26">
         <v>1387.03</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="26">
         <v>56</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="26">
         <v>21956</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="26">
         <v>8.2699999999999996E-2</v>
       </c>
-      <c r="L23" t="s">
+      <c r="L23" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="26">
         <v>0.75</v>
       </c>
-      <c r="N23">
+      <c r="N23" s="26">
         <v>2.6360000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="A24" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="B24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24">
+      <c r="B24" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="26">
         <v>2</v>
       </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="F24" t="s">
+      <c r="D24" s="26">
+        <v>0</v>
+      </c>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="26">
         <v>243</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="26">
         <v>1308.4000000000001</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="26">
         <v>56</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="26">
         <v>23416</v>
       </c>
-      <c r="K24">
+      <c r="K24" s="26">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="L24" t="s">
+      <c r="L24" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="M24">
+      <c r="M24" s="26">
         <v>0.72</v>
       </c>
-      <c r="N24">
+      <c r="N24" s="26">
         <v>2.976</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="A25" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="B25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25">
+      <c r="B25" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="26">
         <v>3</v>
       </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="D25" s="26">
+        <v>0</v>
+      </c>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="26">
         <v>197</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="26">
         <v>1619.34</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="26">
         <v>56</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="26">
         <v>17576</v>
       </c>
-      <c r="K25">
+      <c r="K25" s="26">
         <v>6.4699999999999994E-2</v>
       </c>
-      <c r="L25" t="s">
+      <c r="L25" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="M25">
+      <c r="M25" s="26">
         <v>0.46</v>
       </c>
-      <c r="N25">
+      <c r="N25" s="26">
         <v>2.8119999999999998</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="A26" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="B26" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26">
+      <c r="B26" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="26">
         <v>4</v>
       </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="D26" s="26">
+        <v>0</v>
+      </c>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="26">
         <v>237</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="26">
         <v>1350.95</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="26">
         <v>56</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="26">
         <v>8816</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="26">
         <v>6.4100000000000004E-2</v>
       </c>
-      <c r="L26" t="s">
+      <c r="L26" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="26">
         <v>0.61</v>
       </c>
-      <c r="N26">
+      <c r="N26" s="26">
         <v>3.36</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="A27" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="B27" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27">
+      <c r="B27" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="26">
         <v>5</v>
       </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="F27" t="s">
+      <c r="D27" s="26">
+        <v>0</v>
+      </c>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="26">
         <v>238</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="26">
         <v>1332.38</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="26">
         <v>56</v>
       </c>
-      <c r="J27">
+      <c r="J27" s="26">
         <v>11736</v>
       </c>
-      <c r="K27">
+      <c r="K27" s="26">
         <v>7.22E-2</v>
       </c>
-      <c r="L27" t="s">
+      <c r="L27" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="M27">
+      <c r="M27" s="26">
         <v>0.84</v>
       </c>
-      <c r="N27">
+      <c r="N27" s="26">
         <v>3.0830000000000002</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="A28" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="B28" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28">
+      <c r="B28" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="26">
         <v>6</v>
       </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="F28" t="s">
+      <c r="D28" s="26">
+        <v>0</v>
+      </c>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="26">
         <v>246</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="26">
         <v>1306.56</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="26">
         <v>56</v>
       </c>
-      <c r="J28">
+      <c r="J28" s="26">
         <v>8816</v>
       </c>
-      <c r="K28">
+      <c r="K28" s="26">
         <v>8.0199999999999994E-2</v>
       </c>
-      <c r="L28" t="s">
+      <c r="L28" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="M28">
+      <c r="M28" s="26">
         <v>0.69</v>
       </c>
-      <c r="N28">
+      <c r="N28" s="26">
         <v>2.86</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="A29" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="B29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29">
+      <c r="B29" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="26">
         <v>7</v>
       </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="F29" t="s">
+      <c r="D29" s="26">
+        <v>0</v>
+      </c>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="26">
         <v>242</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="26">
         <v>1316.47</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="26">
         <v>56</v>
       </c>
-      <c r="J29">
+      <c r="J29" s="26">
         <v>8816</v>
       </c>
-      <c r="K29">
+      <c r="K29" s="26">
         <v>7.0400000000000004E-2</v>
       </c>
-      <c r="L29" t="s">
+      <c r="L29" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="M29">
+      <c r="M29" s="26">
         <v>0.48</v>
       </c>
-      <c r="N29">
+      <c r="N29" s="26">
         <v>3.1059999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="A30" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="B30" t="s">
-        <v>15</v>
-      </c>
-      <c r="C30">
+      <c r="B30" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="26">
         <v>8</v>
       </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="F30" t="s">
+      <c r="D30" s="26">
+        <v>0</v>
+      </c>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="26">
         <v>263</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="26">
         <v>1229.48</v>
       </c>
-      <c r="I30">
+      <c r="I30" s="26">
         <v>56</v>
       </c>
-      <c r="J30">
+      <c r="J30" s="26">
         <v>8816</v>
       </c>
-      <c r="K30">
+      <c r="K30" s="26">
         <v>7.7299999999999994E-2</v>
       </c>
-      <c r="L30" t="s">
+      <c r="L30" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="M30">
+      <c r="M30" s="26">
         <v>0.72</v>
       </c>
-      <c r="N30">
+      <c r="N30" s="26">
         <v>2.92</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="A31" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="B31" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31">
+      <c r="B31" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="26">
         <v>9</v>
       </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="F31" t="s">
+      <c r="D31" s="26">
+        <v>0</v>
+      </c>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="26">
         <v>252</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="26">
         <v>1276.3900000000001</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="26">
         <v>56</v>
       </c>
-      <c r="J31">
+      <c r="J31" s="26">
         <v>7356</v>
       </c>
-      <c r="K31">
+      <c r="K31" s="26">
         <v>5.67E-2</v>
       </c>
-      <c r="L31" t="s">
+      <c r="L31" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="M31">
+      <c r="M31" s="26">
         <v>0.79</v>
       </c>
-      <c r="N31">
+      <c r="N31" s="26">
         <v>4.1980000000000004</v>
       </c>
     </row>

</xml_diff>